<commit_message>
Refresh & env added
</commit_message>
<xml_diff>
--- a/FORMS/virtual/students.xlsx
+++ b/FORMS/virtual/students.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,62 +544,222 @@
           <t>S</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1/7/24</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>324243</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Judaism</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>7th</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20240108221909</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Ms.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1/8/24</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Sikhism</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>EE</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>7th</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>20240108222332</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sayantan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Mr.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1/7/24</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>324243</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Judaism</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>CSE</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>7th</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1/8/24</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Jainism</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>ST</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>